<commit_message>
Agrego imagenes de Zin y ya esta
</commit_message>
<xml_diff>
--- a/Ex4/Mediciones/Derivador/IMPbodedermedido.xlsx
+++ b/Ex4/Mediciones/Derivador/IMPbodedermedido.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\milto\Documents\GitHub\TP02\Ex4\Mediciones\Derivador\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E57C4703-BC38-47DA-A166-F6598814F2DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68FE992B-EF19-47AE-BF03-0C68DDBF2F59}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{719BF5D3-7D16-4810-B3EE-22F17955C1CC}"/>
   </bookViews>
@@ -383,7 +383,7 @@
   <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C39"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>